<commit_message>
Work on cash book and id card almost done around 90%
</commit_message>
<xml_diff>
--- a/RICEFW_STATUS.xlsx
+++ b/RICEFW_STATUS.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="38">
   <si>
     <t xml:space="preserve">Type </t>
   </si>
@@ -101,9 +101,6 @@
     <t>Based on filter(i.e. academic program,term)eg-MBA01,1201</t>
   </si>
   <si>
-    <t>Done</t>
-  </si>
-  <si>
     <t>PRODUCTION</t>
   </si>
   <si>
@@ -113,13 +110,34 @@
     <t>Detailed record according to academic program,term eg-bus,hostel,course fees</t>
   </si>
   <si>
-    <t>InProgress</t>
-  </si>
-  <si>
     <t>NO</t>
   </si>
   <si>
     <t>Detailed Student balance record</t>
+  </si>
+  <si>
+    <t>ID Card</t>
+  </si>
+  <si>
+    <t>SRMU student id card</t>
+  </si>
+  <si>
+    <t>psotGoLive</t>
+  </si>
+  <si>
+    <t>WIP</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>Cash Book Summary</t>
+  </si>
+  <si>
+    <t>To print cash book between 2 particular dates (i.e. from date and to date)</t>
+  </si>
+  <si>
+    <t>REports</t>
   </si>
 </sst>
 </file>
@@ -446,10 +464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O5"/>
+  <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -510,7 +528,7 @@
         <v>8</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -545,16 +563,25 @@
         <v>17</v>
       </c>
       <c r="M4" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="N4" t="s">
         <v>18</v>
       </c>
       <c r="O4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
       <c r="F5" t="s">
         <v>13</v>
       </c>
@@ -565,22 +592,98 @@
         <v>15</v>
       </c>
       <c r="I5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="J5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L5" t="s">
         <v>17</v>
       </c>
       <c r="M5" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="N5" t="s">
         <v>18</v>
       </c>
       <c r="O5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" t="s">
         <v>30</v>
+      </c>
+      <c r="J6" t="s">
+        <v>31</v>
+      </c>
+      <c r="L6" t="s">
+        <v>32</v>
+      </c>
+      <c r="M6" t="s">
+        <v>33</v>
+      </c>
+      <c r="N6" t="s">
+        <v>18</v>
+      </c>
+      <c r="O6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I7" t="s">
+        <v>35</v>
+      </c>
+      <c r="J7" t="s">
+        <v>36</v>
+      </c>
+      <c r="L7" t="s">
+        <v>17</v>
+      </c>
+      <c r="M7" t="s">
+        <v>34</v>
+      </c>
+      <c r="N7" t="s">
+        <v>18</v>
+      </c>
+      <c r="O7" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>